<commit_message>
Added test data for official_hca_publication field.
</commit_message>
<xml_diff>
--- a/Schema_Test_Data.xlsx
+++ b/Schema_Test_Data.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/wteh/Documents/GitHub_Issues/Estimated_cell_count/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/enrique/Downloads/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{B5F845C0-ED25-BF45-B243-E51FFBECA8E7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E8BF8731-9593-3C45-B41A-60E1682C5E07}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="10380" yWindow="1680" windowWidth="40820" windowHeight="24280" activeTab="9" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="28800" yWindow="460" windowWidth="38400" windowHeight="21140" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Project" sheetId="1" r:id="rId1"/>
@@ -43,7 +43,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1643" uniqueCount="1025">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1648" uniqueCount="1029">
   <si>
     <t>PROJECT LABEL (Required)</t>
   </si>
@@ -3120,6 +3120,18 @@
   </si>
   <si>
     <t>10x 3' v3</t>
+  </si>
+  <si>
+    <t>OFFICIAL HCA PUBLICATION</t>
+  </si>
+  <si>
+    <t>Has the publication been accepted as an official HCA publication, according to the process described in https://www.humancellatlas.org/publications/ ?</t>
+  </si>
+  <si>
+    <t>Should be one of: yes, or no</t>
+  </si>
+  <si>
+    <t>project.publications.official_hca_publication</t>
   </si>
 </sst>
 </file>
@@ -3802,7 +3814,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-1500-000000000000}">
   <dimension ref="A1:AY11"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="F3" zoomScale="79" zoomScaleNormal="79" workbookViewId="0">
+    <sheetView topLeftCell="F3" zoomScale="79" zoomScaleNormal="79" workbookViewId="0">
       <selection activeCell="Q6" sqref="Q6"/>
     </sheetView>
   </sheetViews>
@@ -6328,10 +6340,10 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
-  <dimension ref="A1:E6"/>
+  <dimension ref="A1:F7"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="C7" sqref="C7"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="I6" sqref="I6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -6340,9 +6352,10 @@
     <col min="2" max="2" width="28.6640625" customWidth="1"/>
     <col min="3" max="4" width="25.6640625" customWidth="1"/>
     <col min="5" max="5" width="59" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="41.1640625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" ht="30" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:6" ht="30" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A1" s="1" t="s">
         <v>84</v>
       </c>
@@ -6358,8 +6371,11 @@
       <c r="E1" s="1" t="s">
         <v>100</v>
       </c>
-    </row>
-    <row r="2" spans="1:5" ht="51" x14ac:dyDescent="0.2">
+      <c r="F1" s="1" t="s">
+        <v>1025</v>
+      </c>
+    </row>
+    <row r="2" spans="1:6" ht="340" x14ac:dyDescent="0.2">
       <c r="A2" s="2" t="s">
         <v>85</v>
       </c>
@@ -6375,8 +6391,11 @@
       <c r="E2" s="2" t="s">
         <v>101</v>
       </c>
-    </row>
-    <row r="3" spans="1:5" ht="51" x14ac:dyDescent="0.2">
+      <c r="F2" s="2" t="s">
+        <v>1026</v>
+      </c>
+    </row>
+    <row r="3" spans="1:6" ht="68" x14ac:dyDescent="0.2">
       <c r="A3" s="2" t="s">
         <v>86</v>
       </c>
@@ -6392,8 +6411,11 @@
       <c r="E3" s="2" t="s">
         <v>102</v>
       </c>
-    </row>
-    <row r="4" spans="1:5" hidden="1" x14ac:dyDescent="0.2">
+      <c r="F3" s="2" t="s">
+        <v>1027</v>
+      </c>
+    </row>
+    <row r="4" spans="1:6" ht="24" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A4" s="3" t="s">
         <v>87</v>
       </c>
@@ -6409,8 +6431,11 @@
       <c r="E4" s="3" t="s">
         <v>103</v>
       </c>
-    </row>
-    <row r="5" spans="1:5" ht="30" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="F4" s="3" t="s">
+        <v>1028</v>
+      </c>
+    </row>
+    <row r="5" spans="1:6" ht="30" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A5" s="1" t="s">
         <v>4</v>
       </c>
@@ -6418,8 +6443,9 @@
       <c r="C5" s="1"/>
       <c r="D5" s="1"/>
       <c r="E5" s="1"/>
-    </row>
-    <row r="6" spans="1:5" ht="48" x14ac:dyDescent="0.2">
+      <c r="F5" s="1"/>
+    </row>
+    <row r="6" spans="1:6" ht="48" x14ac:dyDescent="0.2">
       <c r="A6" t="s">
         <v>886</v>
       </c>
@@ -6432,6 +6458,12 @@
       <c r="E6" s="4" t="s">
         <v>965</v>
       </c>
+      <c r="F6" s="3" t="s">
+        <v>855</v>
+      </c>
+    </row>
+    <row r="7" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="F7" s="3"/>
     </row>
   </sheetData>
   <hyperlinks>

</xml_diff>

<commit_message>
Update test data for release-data-09/02/2022
</commit_message>
<xml_diff>
--- a/Schema_Test_Data.xlsx
+++ b/Schema_Test_Data.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/wteh/Documents/Wrangling/Schema-test-data/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/wteh/Downloads/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E76E4084-D9A9-D046-A140-C60B16468AD7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="8_{50A5C63E-7107-AD43-96C5-A397DE55E333}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="7920" yWindow="1840" windowWidth="30640" windowHeight="23360" firstSheet="8" activeTab="13" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="500" windowWidth="28800" windowHeight="16080" firstSheet="1" activeTab="4" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Project" sheetId="1" r:id="rId1"/>
@@ -48,7 +48,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2251" uniqueCount="1251">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2255" uniqueCount="1251">
   <si>
     <t>PROJECT LABEL (Required)</t>
   </si>
@@ -6381,7 +6381,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-1500-000000000000}">
   <dimension ref="A1:BC11"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A2" zoomScale="79" zoomScaleNormal="79" workbookViewId="0">
+    <sheetView topLeftCell="A2" zoomScale="79" zoomScaleNormal="79" workbookViewId="0">
       <selection activeCell="C3" sqref="C3"/>
     </sheetView>
   </sheetViews>
@@ -10101,8 +10101,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0400-000000000000}">
   <dimension ref="A1:BW28"/>
   <sheetViews>
-    <sheetView topLeftCell="F1" workbookViewId="0">
-      <selection activeCell="P8" sqref="P8:BC8"/>
+    <sheetView tabSelected="1" topLeftCell="Z2" workbookViewId="0">
+      <selection activeCell="AD3" sqref="AD3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -11171,7 +11171,12 @@
       <c r="AB6" t="s">
         <v>858</v>
       </c>
-      <c r="AD6" s="3"/>
+      <c r="AC6" t="s">
+        <v>968</v>
+      </c>
+      <c r="AD6" s="3" t="s">
+        <v>858</v>
+      </c>
     </row>
     <row r="7" spans="1:75" x14ac:dyDescent="0.2">
       <c r="A7" s="7" t="s">
@@ -11222,8 +11227,12 @@
       <c r="AB7" t="s">
         <v>858</v>
       </c>
-      <c r="AC7" s="3"/>
-      <c r="AD7" s="3"/>
+      <c r="AC7" s="3" t="s">
+        <v>968</v>
+      </c>
+      <c r="AD7" s="3" t="s">
+        <v>858</v>
+      </c>
     </row>
     <row r="8" spans="1:75" x14ac:dyDescent="0.2">
       <c r="A8" s="7" t="s">
@@ -12059,8 +12068,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0500-000000000000}">
   <dimension ref="A1:BH8"/>
   <sheetViews>
-    <sheetView topLeftCell="AQ1" workbookViewId="0">
-      <selection activeCell="AR9" sqref="AR9"/>
+    <sheetView topLeftCell="AO2" workbookViewId="0">
+      <selection activeCell="AQ9" sqref="AQ9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -13005,7 +13014,7 @@
         <v>858</v>
       </c>
       <c r="AQ8" s="7" t="s">
-        <v>852</v>
+        <v>1247</v>
       </c>
       <c r="AR8" s="3" t="s">
         <v>966</v>
@@ -13394,7 +13403,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{0EB3A245-B994-8A41-A981-DAC8129A1EA8}">
   <dimension ref="A1:AF6"/>
   <sheetViews>
-    <sheetView topLeftCell="H1" workbookViewId="0">
+    <sheetView topLeftCell="H2" workbookViewId="0">
       <selection activeCell="O7" sqref="O7"/>
     </sheetView>
   </sheetViews>

</xml_diff>